<commit_message>
Update fuzzy membership parameters and add table of contents to report; adjust workspace paths
</commit_message>
<xml_diff>
--- a/wykresy.xlsx
+++ b/wykresy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\STUDIA_FOLDERY\analizy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Pulpit\analizy-przestrzenne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E0879C-E19E-452E-81E0-ACB16B345346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC71EB-6128-4C0B-AE36-1831725FD56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{9EF8476E-6667-45BC-BC00-D969981DDBE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{9EF8476E-6667-45BC-BC00-D969981DDBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="kryterium 1" sheetId="1" r:id="rId1"/>
@@ -966,13 +966,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3000</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6000</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,7 +1020,7 @@
         <c:axId val="1703879295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10000"/>
+          <c:max val="100"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1060,7 +1060,19 @@
                   <a:rPr lang="pl-PL" b="1">
                     <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>odległość od węzła drogowego [m]</a:t>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" b="1" baseline="0">
+                    <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> maksymalnej </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" b="1">
+                    <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>odległości od węzła drogowego</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1105,7 +1117,7 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
-            <a:tailEnd type="triangle"/>
+            <a:tailEnd type="none"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1132,7 +1144,7 @@
         <c:crossAx val="1703878815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1000"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1703878815"/>
@@ -2149,7 +2161,7 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
@@ -2404,7 +2416,7 @@
             </a:solidFill>
             <a:round/>
             <a:headEnd type="none"/>
-            <a:tailEnd type="triangle"/>
+            <a:tailEnd type="none"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2539,10 +2551,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2590,7 +2602,8 @@
         <c:axId val="1703879295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="200"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2713,7 +2726,7 @@
         <c:crossAx val="1703878815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1703878815"/>
@@ -2937,13 +2950,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2991,7 +3004,7 @@
         <c:axId val="1703879295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3030,8 +3043,17 @@
                   <a:rPr lang="pl-PL" b="1">
                     <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>liczba kilometrów dróg utwardzonych na km² powierzchni</a:t>
+                  <a:t>% maksymalnej gęstości</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" b="1" baseline="0">
+                    <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> dróg w obszarze</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" b="1">
+                  <a:latin typeface="Century Schoolbook" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3102,7 +3124,7 @@
         <c:crossAx val="1703878815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1703878815"/>
@@ -3326,13 +3348,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3380,7 +3402,7 @@
         <c:axId val="1703879295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
+          <c:max val="15"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3492,7 +3514,7 @@
         <c:crossAx val="1703878815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="4"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1703878815"/>
@@ -3584,7 +3606,7 @@
             </a:solidFill>
             <a:round/>
             <a:headEnd type="none"/>
-            <a:tailEnd type="triangle"/>
+            <a:tailEnd type="none"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -10611,15 +10633,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1795671</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:colOff>468894</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>51841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>125895</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>170328</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53790</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10648,16 +10670,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1801906</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>591671</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>53788</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>172667</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1577789</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>170330</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10691,16 +10713,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19371</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10734,16 +10756,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>126051</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10777,15 +10799,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>118431</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10863,16 +10885,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>401618</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>64546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>515918</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>34611</xdr:rowOff>
+      <xdr:rowOff>7717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10988,8 +11010,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>75848</xdr:rowOff>
     </xdr:to>
@@ -11340,8 +11362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C6F23A-0ACE-4A99-AC0C-F32DB29AF5F9}">
   <dimension ref="B3:H32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11503,8 +11525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AACA60C-D287-4B43-A448-EEC66974A74D}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11539,7 +11561,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -11564,7 +11586,7 @@
   <dimension ref="C3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11598,7 +11620,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -11606,7 +11628,7 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -11623,7 +11645,7 @@
   <dimension ref="C3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11649,7 +11671,7 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -11657,7 +11679,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -11665,7 +11687,7 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -11682,7 +11704,7 @@
   <dimension ref="C3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11709,7 +11731,7 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -11717,7 +11739,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -11725,7 +11747,7 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -11742,7 +11764,7 @@
   <dimension ref="C3:Q25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11888,7 +11910,7 @@
   <dimension ref="C3:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11915,7 +11937,7 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -11923,7 +11945,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>6000</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -11931,7 +11953,7 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>0</v>

</xml_diff>

<commit_message>
Add cost calculation and pathfinding logic in analysis; update main function and adjust table of contents
</commit_message>
<xml_diff>
--- a/wykresy.xlsx
+++ b/wykresy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Pulpit\analizy-przestrzenne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\STUDIA_FOLDERY\analizy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC71EB-6128-4C0B-AE36-1831725FD56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CB6DD-96F5-42C1-931C-49132AC0C7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{9EF8476E-6667-45BC-BC00-D969981DDBE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="6" xr2:uid="{9EF8476E-6667-45BC-BC00-D969981DDBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="kryterium 1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>225</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>270</c:v>
@@ -966,10 +966,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>100</c:v>
@@ -3741,10 +3741,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>135</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>225</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>270</c:v>
@@ -3916,7 +3916,7 @@
         <c:crossAx val="1703878815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="45"/>
+        <c:majorUnit val="22.5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1703878815"/>
@@ -4143,7 +4143,7 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>135</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>360</c:v>
@@ -10886,15 +10886,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>401618</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>64546</xdr:rowOff>
+      <xdr:colOff>43030</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>73511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>515918</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>7717</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>170330</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>16681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10923,16 +10923,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>296732</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>98164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>179391</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>591670</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44921</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11764,7 +11764,7 @@
   <dimension ref="C3:Q25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11817,13 +11817,13 @@
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -11831,7 +11831,7 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -11877,7 +11877,7 @@
     </row>
     <row r="23" spans="16:17" x14ac:dyDescent="0.3">
       <c r="P23">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -11910,7 +11910,7 @@
   <dimension ref="C3:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11937,7 +11937,7 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -11945,7 +11945,7 @@
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>0</v>

</xml_diff>